<commit_message>
Reading data from Excel files refined and tested
</commit_message>
<xml_diff>
--- a/inst/extdata/easy_data.xlsx
+++ b/inst/extdata/easy_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CE73CD-3682-4B20-8072-255C4F30210D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E302F61-5B55-42C0-8B07-F5442D2BF677}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9156" yWindow="6636" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="4068" windowWidth="20244" windowHeight="16464" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
-    <t>Injection</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>(123.45; 678)</t>
+  </si>
+  <si>
+    <t>Injection_order</t>
   </si>
 </sst>
 </file>
@@ -409,14 +409,14 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -455,98 +455,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>9</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>10</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>11</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>12</v>
       </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -557,7 +557,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>50000</v>
@@ -567,7 +567,7 @@
         <v>51000</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:Q4" si="0">F4+1000</f>
+        <f t="shared" ref="G4:P4" si="0">F4+1000</f>
         <v>52000</v>
       </c>
       <c r="H4">
@@ -607,7 +607,7 @@
         <v>61000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>A4+1</f>
         <v>2</v>
@@ -625,7 +625,7 @@
         <v>47000</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:Q5" si="1">E5+1000</f>
+        <f t="shared" ref="F5:P5" si="1">E5+1000</f>
         <v>48000</v>
       </c>
       <c r="G5">
@@ -669,7 +669,7 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ref="A6:A13" si="2">A5+1</f>
         <v>3</v>
@@ -687,7 +687,7 @@
         <v>44000</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:Q6" si="6">E6+1000</f>
+        <f t="shared" ref="F6:P6" si="6">E6+1000</f>
         <v>45000</v>
       </c>
       <c r="G6">
@@ -731,7 +731,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -749,7 +749,7 @@
         <v>41000</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:Q7" si="7">E7+1000</f>
+        <f t="shared" ref="F7:P7" si="7">E7+1000</f>
         <v>42000</v>
       </c>
       <c r="G7">
@@ -793,7 +793,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -811,7 +811,7 @@
         <v>38000</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:Q8" si="8">E8+1000</f>
+        <f t="shared" ref="F8:P8" si="8">E8+1000</f>
         <v>39000</v>
       </c>
       <c r="G8">
@@ -855,7 +855,7 @@
         <v>49000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -873,7 +873,7 @@
         <v>35000</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:Q9" si="9">E9+1000</f>
+        <f t="shared" ref="F9:P9" si="9">E9+1000</f>
         <v>36000</v>
       </c>
       <c r="G9">
@@ -917,7 +917,7 @@
         <v>46000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -935,7 +935,7 @@
         <v>32000</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:Q10" si="10">E10+1000</f>
+        <f t="shared" ref="F10:P10" si="10">E10+1000</f>
         <v>33000</v>
       </c>
       <c r="G10">
@@ -979,7 +979,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -997,7 +997,7 @@
         <v>29000</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:Q11" si="11">E11+1000</f>
+        <f t="shared" ref="F11:P11" si="11">E11+1000</f>
         <v>30000</v>
       </c>
       <c r="G11">
@@ -1041,7 +1041,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1059,7 +1059,7 @@
         <v>26000</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:Q12" si="12">E12+1000</f>
+        <f t="shared" ref="F12:P12" si="12">E12+1000</f>
         <v>27000</v>
       </c>
       <c r="G12">
@@ -1103,7 +1103,7 @@
         <v>37000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1121,7 +1121,7 @@
         <v>23000</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:Q13" si="13">E13+1000</f>
+        <f t="shared" ref="F13:P13" si="13">E13+1000</f>
         <v>24000</v>
       </c>
       <c r="G13">

</xml_diff>

<commit_message>
results field removed from Metabosets, the results are now in featureData
</commit_message>
<xml_diff>
--- a/inst/extdata/easy_data.xlsx
+++ b/inst/extdata/easy_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E302F61-5B55-42C0-8B07-F5442D2BF677}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B04B6A7-F6F6-4AD6-A639-1BF0A6E87290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="4068" windowWidth="20244" windowHeight="16464" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="2748" windowWidth="26136" windowHeight="16284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Group</t>
   </si>
@@ -89,6 +91,12 @@
   </si>
   <si>
     <t>Injection_order</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -406,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,670 +505,711 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>7</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L4" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M4" t="s">
         <v>9</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N4" t="s">
         <v>10</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O4" t="s">
         <v>11</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>50</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>50000</v>
       </c>
-      <c r="F4">
-        <f>E4+1000</f>
+      <c r="F5">
+        <f>E5+1000</f>
         <v>51000</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4:P4" si="0">F4+1000</f>
+      <c r="G5">
+        <f t="shared" ref="G5:P5" si="0">F5+1000</f>
         <v>52000</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>53000</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>54000</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>55000</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>56000</v>
       </c>
-      <c r="L4">
+      <c r="L5">
         <f t="shared" si="0"/>
         <v>57000</v>
       </c>
-      <c r="M4">
+      <c r="M5">
         <f t="shared" si="0"/>
         <v>58000</v>
       </c>
-      <c r="N4">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>59000</v>
       </c>
-      <c r="O4">
+      <c r="O5">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="P4">
+      <c r="P5">
         <f t="shared" si="0"/>
         <v>61000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f>A4+1</f>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B5">
-        <f>B4+50</f>
+      <c r="B6">
+        <f>B5+50</f>
         <v>100</v>
       </c>
-      <c r="C5">
-        <f>C4+0.5</f>
+      <c r="C6">
+        <f>C5+0.5</f>
         <v>1</v>
       </c>
-      <c r="E5">
-        <f>E4-3000</f>
+      <c r="E6">
+        <f>E5-3000</f>
         <v>47000</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:P5" si="1">E5+1000</f>
+      <c r="F6">
+        <f t="shared" ref="F6:P6" si="1">E6+1000</f>
         <v>48000</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>49000</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>50000</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>51000</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <f t="shared" si="1"/>
         <v>52000</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>53000</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <f t="shared" si="1"/>
         <v>54000</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <f t="shared" si="1"/>
         <v>55000</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <f t="shared" si="1"/>
         <v>56000</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <f t="shared" si="1"/>
         <v>57000</v>
       </c>
-      <c r="P5">
+      <c r="P6">
         <f t="shared" si="1"/>
         <v>58000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" ref="A6:A13" si="2">A5+1</f>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" ref="A7:A14" si="2">A6+1</f>
         <v>3</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B13" si="3">B5+50</f>
+      <c r="B7">
+        <f t="shared" ref="B7:B14" si="3">B6+50</f>
         <v>150</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C13" si="4">C5+0.5</f>
+      <c r="C7">
+        <f t="shared" ref="C7:C14" si="4">C6+0.5</f>
         <v>1.5</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E13" si="5">E5-3000</f>
+      <c r="E7">
+        <f t="shared" ref="E7:E14" si="5">E6-3000</f>
         <v>44000</v>
       </c>
-      <c r="F6">
-        <f t="shared" ref="F6:P6" si="6">E6+1000</f>
+      <c r="F7">
+        <f t="shared" ref="F7:P7" si="6">E7+1000</f>
         <v>45000</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <f t="shared" si="6"/>
         <v>46000</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <f t="shared" si="6"/>
         <v>47000</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <f t="shared" si="6"/>
         <v>48000</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <f t="shared" si="6"/>
         <v>49000</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <f t="shared" si="6"/>
         <v>50000</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <f t="shared" si="6"/>
         <v>51000</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <f t="shared" si="6"/>
         <v>52000</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <f t="shared" si="6"/>
         <v>53000</v>
       </c>
-      <c r="O6">
+      <c r="O7">
         <f t="shared" si="6"/>
         <v>54000</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <f t="shared" si="6"/>
         <v>55000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="5"/>
-        <v>41000</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:P7" si="7">E7+1000</f>
-        <v>42000</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="7"/>
-        <v>43000</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="7"/>
-        <v>44000</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="7"/>
-        <v>45000</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="7"/>
-        <v>46000</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="7"/>
-        <v>47000</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="7"/>
-        <v>48000</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="7"/>
-        <v>49000</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="7"/>
-        <v>50000</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="7"/>
-        <v>51000</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="7"/>
-        <v>52000</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <f t="shared" si="5"/>
-        <v>38000</v>
+        <v>41000</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:P8" si="8">E8+1000</f>
-        <v>39000</v>
+        <f t="shared" ref="F8:P8" si="7">E8+1000</f>
+        <v>42000</v>
       </c>
       <c r="G8">
-        <f t="shared" si="8"/>
-        <v>40000</v>
+        <f t="shared" si="7"/>
+        <v>43000</v>
       </c>
       <c r="H8">
-        <f t="shared" si="8"/>
-        <v>41000</v>
+        <f t="shared" si="7"/>
+        <v>44000</v>
       </c>
       <c r="I8">
-        <f t="shared" si="8"/>
-        <v>42000</v>
+        <f t="shared" si="7"/>
+        <v>45000</v>
       </c>
       <c r="J8">
-        <f t="shared" si="8"/>
-        <v>43000</v>
+        <f t="shared" si="7"/>
+        <v>46000</v>
       </c>
       <c r="K8">
-        <f t="shared" si="8"/>
-        <v>44000</v>
+        <f t="shared" si="7"/>
+        <v>47000</v>
       </c>
       <c r="L8">
-        <f t="shared" si="8"/>
-        <v>45000</v>
+        <f t="shared" si="7"/>
+        <v>48000</v>
       </c>
       <c r="M8">
-        <f t="shared" si="8"/>
-        <v>46000</v>
+        <f t="shared" si="7"/>
+        <v>49000</v>
       </c>
       <c r="N8">
-        <f t="shared" si="8"/>
-        <v>47000</v>
+        <f t="shared" si="7"/>
+        <v>50000</v>
       </c>
       <c r="O8">
-        <f t="shared" si="8"/>
-        <v>48000</v>
+        <f t="shared" si="7"/>
+        <v>51000</v>
       </c>
       <c r="P8">
-        <f t="shared" si="8"/>
-        <v>49000</v>
+        <f t="shared" si="7"/>
+        <v>52000</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <f t="shared" si="3"/>
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C9">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E9">
         <f t="shared" si="5"/>
-        <v>35000</v>
+        <v>38000</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:P9" si="9">E9+1000</f>
-        <v>36000</v>
+        <f t="shared" ref="F9:P9" si="8">E9+1000</f>
+        <v>39000</v>
       </c>
       <c r="G9">
-        <f t="shared" si="9"/>
-        <v>37000</v>
+        <f t="shared" si="8"/>
+        <v>40000</v>
       </c>
       <c r="H9">
-        <f t="shared" si="9"/>
-        <v>38000</v>
+        <f t="shared" si="8"/>
+        <v>41000</v>
       </c>
       <c r="I9">
-        <f t="shared" si="9"/>
-        <v>39000</v>
+        <f t="shared" si="8"/>
+        <v>42000</v>
       </c>
       <c r="J9">
-        <f t="shared" si="9"/>
-        <v>40000</v>
+        <f t="shared" si="8"/>
+        <v>43000</v>
       </c>
       <c r="K9">
-        <f t="shared" si="9"/>
-        <v>41000</v>
+        <f t="shared" si="8"/>
+        <v>44000</v>
       </c>
       <c r="L9">
-        <f t="shared" si="9"/>
-        <v>42000</v>
+        <f t="shared" si="8"/>
+        <v>45000</v>
       </c>
       <c r="M9">
-        <f t="shared" si="9"/>
-        <v>43000</v>
+        <f t="shared" si="8"/>
+        <v>46000</v>
       </c>
       <c r="N9">
-        <f t="shared" si="9"/>
-        <v>44000</v>
+        <f t="shared" si="8"/>
+        <v>47000</v>
       </c>
       <c r="O9">
-        <f t="shared" si="9"/>
-        <v>45000</v>
+        <f t="shared" si="8"/>
+        <v>48000</v>
       </c>
       <c r="P9">
-        <f t="shared" si="9"/>
-        <v>46000</v>
+        <f t="shared" si="8"/>
+        <v>49000</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <f t="shared" si="3"/>
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f t="shared" si="5"/>
-        <v>32000</v>
+        <v>35000</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:P10" si="10">E10+1000</f>
-        <v>33000</v>
+        <f t="shared" ref="F10:P10" si="9">E10+1000</f>
+        <v>36000</v>
       </c>
       <c r="G10">
-        <f t="shared" si="10"/>
-        <v>34000</v>
+        <f t="shared" si="9"/>
+        <v>37000</v>
       </c>
       <c r="H10">
-        <f t="shared" si="10"/>
-        <v>35000</v>
+        <f t="shared" si="9"/>
+        <v>38000</v>
       </c>
       <c r="I10">
-        <f t="shared" si="10"/>
-        <v>36000</v>
+        <f t="shared" si="9"/>
+        <v>39000</v>
       </c>
       <c r="J10">
-        <f t="shared" si="10"/>
-        <v>37000</v>
+        <f t="shared" si="9"/>
+        <v>40000</v>
       </c>
       <c r="K10">
-        <f t="shared" si="10"/>
-        <v>38000</v>
+        <f t="shared" si="9"/>
+        <v>41000</v>
       </c>
       <c r="L10">
-        <f t="shared" si="10"/>
-        <v>39000</v>
+        <f t="shared" si="9"/>
+        <v>42000</v>
       </c>
       <c r="M10">
-        <f t="shared" si="10"/>
-        <v>40000</v>
+        <f t="shared" si="9"/>
+        <v>43000</v>
       </c>
       <c r="N10">
-        <f t="shared" si="10"/>
-        <v>41000</v>
+        <f t="shared" si="9"/>
+        <v>44000</v>
       </c>
       <c r="O10">
-        <f t="shared" si="10"/>
-        <v>42000</v>
+        <f t="shared" si="9"/>
+        <v>45000</v>
       </c>
       <c r="P10">
-        <f t="shared" si="10"/>
-        <v>43000</v>
+        <f t="shared" si="9"/>
+        <v>46000</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <f t="shared" si="3"/>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="C11">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="E11">
         <f t="shared" si="5"/>
-        <v>29000</v>
+        <v>32000</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:P11" si="11">E11+1000</f>
-        <v>30000</v>
+        <f t="shared" ref="F11:P11" si="10">E11+1000</f>
+        <v>33000</v>
       </c>
       <c r="G11">
-        <f t="shared" si="11"/>
-        <v>31000</v>
+        <f t="shared" si="10"/>
+        <v>34000</v>
       </c>
       <c r="H11">
-        <f t="shared" si="11"/>
-        <v>32000</v>
+        <f t="shared" si="10"/>
+        <v>35000</v>
       </c>
       <c r="I11">
-        <f t="shared" si="11"/>
-        <v>33000</v>
+        <f t="shared" si="10"/>
+        <v>36000</v>
       </c>
       <c r="J11">
-        <f t="shared" si="11"/>
-        <v>34000</v>
+        <f t="shared" si="10"/>
+        <v>37000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="11"/>
-        <v>35000</v>
+        <f t="shared" si="10"/>
+        <v>38000</v>
       </c>
       <c r="L11">
-        <f t="shared" si="11"/>
-        <v>36000</v>
+        <f t="shared" si="10"/>
+        <v>39000</v>
       </c>
       <c r="M11">
-        <f t="shared" si="11"/>
-        <v>37000</v>
+        <f t="shared" si="10"/>
+        <v>40000</v>
       </c>
       <c r="N11">
-        <f t="shared" si="11"/>
-        <v>38000</v>
+        <f t="shared" si="10"/>
+        <v>41000</v>
       </c>
       <c r="O11">
-        <f t="shared" si="11"/>
-        <v>39000</v>
+        <f t="shared" si="10"/>
+        <v>42000</v>
       </c>
       <c r="P11">
-        <f t="shared" si="11"/>
-        <v>40000</v>
+        <f t="shared" si="10"/>
+        <v>43000</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <f t="shared" si="3"/>
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="C12">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <f t="shared" si="5"/>
-        <v>26000</v>
+        <v>29000</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:P12" si="12">E12+1000</f>
-        <v>27000</v>
+        <f t="shared" ref="F12:P12" si="11">E12+1000</f>
+        <v>30000</v>
       </c>
       <c r="G12">
-        <f t="shared" si="12"/>
-        <v>28000</v>
+        <f t="shared" si="11"/>
+        <v>31000</v>
       </c>
       <c r="H12">
-        <f t="shared" si="12"/>
-        <v>29000</v>
+        <f t="shared" si="11"/>
+        <v>32000</v>
       </c>
       <c r="I12">
-        <f t="shared" si="12"/>
-        <v>30000</v>
+        <f t="shared" si="11"/>
+        <v>33000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="12"/>
-        <v>31000</v>
+        <f t="shared" si="11"/>
+        <v>34000</v>
       </c>
       <c r="K12">
-        <f t="shared" si="12"/>
-        <v>32000</v>
+        <f t="shared" si="11"/>
+        <v>35000</v>
       </c>
       <c r="L12">
-        <f t="shared" si="12"/>
-        <v>33000</v>
+        <f t="shared" si="11"/>
+        <v>36000</v>
       </c>
       <c r="M12">
-        <f t="shared" si="12"/>
-        <v>34000</v>
+        <f t="shared" si="11"/>
+        <v>37000</v>
       </c>
       <c r="N12">
-        <f t="shared" si="12"/>
-        <v>35000</v>
+        <f t="shared" si="11"/>
+        <v>38000</v>
       </c>
       <c r="O12">
-        <f t="shared" si="12"/>
-        <v>36000</v>
+        <f t="shared" si="11"/>
+        <v>39000</v>
       </c>
       <c r="P12">
-        <f t="shared" si="12"/>
-        <v>37000</v>
+        <f t="shared" si="11"/>
+        <v>40000</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="E13">
         <f t="shared" si="5"/>
+        <v>26000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:P13" si="12">E13+1000</f>
+        <v>27000</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="12"/>
+        <v>28000</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="12"/>
+        <v>29000</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="12"/>
+        <v>30000</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="12"/>
+        <v>31000</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="12"/>
+        <v>32000</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="12"/>
+        <v>33000</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="12"/>
+        <v>34000</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="12"/>
+        <v>35000</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="12"/>
+        <v>36000</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="12"/>
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="5"/>
         <v>23000</v>
       </c>
-      <c r="F13">
-        <f t="shared" ref="F13:P13" si="13">E13+1000</f>
+      <c r="F14">
+        <f t="shared" ref="F14:P14" si="13">E14+1000</f>
         <v>24000</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <f t="shared" si="13"/>
         <v>25000</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <f t="shared" si="13"/>
         <v>26000</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <f t="shared" si="13"/>
         <v>27000</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <f t="shared" si="13"/>
         <v>28000</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <f t="shared" si="13"/>
         <v>29000</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <f t="shared" si="13"/>
         <v>30000</v>
       </c>
-      <c r="M13">
+      <c r="M14">
         <f t="shared" si="13"/>
         <v>31000</v>
       </c>
-      <c r="N13">
+      <c r="N14">
         <f t="shared" si="13"/>
         <v>32000</v>
       </c>
-      <c r="O13">
+      <c r="O14">
         <f t="shared" si="13"/>
         <v>33000</v>
       </c>
-      <c r="P13">
+      <c r="P14">
         <f t="shared" si="13"/>
         <v>34000</v>
       </c>

</xml_diff>